<commit_message>
Ajustes na planilha de dados
</commit_message>
<xml_diff>
--- a/pages/PLANTA_DE_PRODUÇÃO(FIOS_INDUSTRIAIS).xlsx
+++ b/pages/PLANTA_DE_PRODUÇÃO(FIOS_INDUSTRIAIS).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\PLANEJAMENTO\Gustavo Moraes\01 - Estudos\Work-Paramount\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\PLANEJAMENTO\Gustavo Moraes\01 - Estudos\Work-Paramount\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83943715-6CC4-47CB-ADCD-ED6C45C05B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B11DE6F-99A7-4787-84A1-A32E44DAB5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{46F42DF5-A9D7-49AF-BA20-293A78FB7E78}"/>
   </bookViews>
@@ -979,12 +979,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1057,7 +1058,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1077,8 +1078,9 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1256,8 +1258,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{32C6F1E6-1D70-4994-98C3-EC9A80334A19}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{1CFDBA2B-A08C-46AA-9F9B-F7ED8870E843}"/>
@@ -1267,6 +1275,7 @@
     <cellStyle name="Vírgula 2 2 2" xfId="17" xr:uid="{F0EBA0FF-2FE7-4FDB-8F1E-491985A09383}"/>
     <cellStyle name="Vírgula 2 3" xfId="10" xr:uid="{2BD088E9-707B-473B-B595-84CD6E211392}"/>
     <cellStyle name="Vírgula 2 4" xfId="14" xr:uid="{65D2538B-870E-443C-8F93-1A5D743B8F7E}"/>
+    <cellStyle name="Vírgula 2 5" xfId="19" xr:uid="{EABEBC4E-9ACE-4DAC-A2B7-A3661FE13FC2}"/>
     <cellStyle name="Vírgula 3" xfId="5" xr:uid="{414D4A6A-C812-4E1F-BAAE-9F830F0AA327}"/>
     <cellStyle name="Vírgula 3 2" xfId="8" xr:uid="{508427C5-AC80-453D-A144-2CF24BB964D0}"/>
     <cellStyle name="Vírgula 3 2 2" xfId="18" xr:uid="{5931373B-77EA-42AD-BC69-4053B876E244}"/>
@@ -1610,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56851730-25A0-448D-A189-DA13E238D33F}">
   <dimension ref="A1:L467"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E310" sqref="E310"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H470" sqref="H470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2664,7 @@
         <v>280</v>
       </c>
       <c r="I26" s="22">
-        <f t="shared" si="0"/>
+        <f>1000/H26</f>
         <v>3.5714285714285716</v>
       </c>
       <c r="J26" s="21" t="s">
@@ -2971,7 +2980,7 @@
       <c r="G34" s="4">
         <v>70</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="55">
         <v>280</v>
       </c>
       <c r="I34" s="22">
@@ -3011,7 +3020,7 @@
       <c r="G35" s="35">
         <v>85</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H35" s="56">
         <v>61.2</v>
       </c>
       <c r="I35" s="22">
@@ -3051,7 +3060,7 @@
       <c r="G36" s="35">
         <v>70</v>
       </c>
-      <c r="H36" s="36">
+      <c r="H36" s="56">
         <v>163.80000000000001</v>
       </c>
       <c r="I36" s="22">
@@ -3091,7 +3100,7 @@
       <c r="G37" s="35">
         <v>80</v>
       </c>
-      <c r="H37" s="36">
+      <c r="H37" s="56">
         <v>124.68705882352943</v>
       </c>
       <c r="I37" s="22">
@@ -3131,7 +3140,7 @@
       <c r="G38" s="35">
         <v>70</v>
       </c>
-      <c r="H38" s="36">
+      <c r="H38" s="56">
         <v>163.80000000000001</v>
       </c>
       <c r="I38" s="22">
@@ -3171,7 +3180,7 @@
       <c r="G39" s="35">
         <v>80</v>
       </c>
-      <c r="H39" s="36">
+      <c r="H39" s="56">
         <v>155.85882352941178</v>
       </c>
       <c r="I39" s="22">
@@ -3211,12 +3220,12 @@
       <c r="G40" s="35">
         <v>82.4</v>
       </c>
-      <c r="H40" s="36">
-        <v>117.59657142857144</v>
+      <c r="H40" s="56">
+        <v>82.317599999999999</v>
       </c>
       <c r="I40" s="22">
         <f t="shared" si="0"/>
-        <v>8.5036492803483092</v>
+        <v>12.148070400497586</v>
       </c>
       <c r="J40" s="18" t="s">
         <v>63</v>
@@ -3226,7 +3235,7 @@
       </c>
       <c r="L40" s="46">
         <f>I40 - Planilha2!I40 / Planilha1!I40</f>
-        <v>7.5036492803483092</v>
+        <v>11.448070400497587</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -3251,12 +3260,12 @@
       <c r="G41" s="35">
         <v>80</v>
       </c>
-      <c r="H41" s="36">
-        <v>123.42857142857143</v>
+      <c r="H41" s="56">
+        <v>96</v>
       </c>
       <c r="I41" s="22">
         <f t="shared" si="0"/>
-        <v>8.1018518518518512</v>
+        <v>10.416666666666666</v>
       </c>
       <c r="J41" s="18" t="s">
         <v>63</v>
@@ -3266,7 +3275,7 @@
       </c>
       <c r="L41" s="46">
         <f>I41 - Planilha2!I41 / Planilha1!I41</f>
-        <v>7.1018518518518512</v>
+        <v>9.6388888888888875</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionando aplicativo para verificar o Roteiro de Produção e outro para verificar a diferença no rendimento das maquinas.
</commit_message>
<xml_diff>
--- a/pages/PLANTA_DE_PRODUÇÃO(FIOS_INDUSTRIAIS).xlsx
+++ b/pages/PLANTA_DE_PRODUÇÃO(FIOS_INDUSTRIAIS).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\PLANEJAMENTO\Gustavo Moraes\01 - Estudos\Work-Paramount\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B11DE6F-99A7-4787-84A1-A32E44DAB5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620A4294-A520-47BF-ABF8-43E7C395CF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{46F42DF5-A9D7-49AF-BA20-293A78FB7E78}"/>
   </bookViews>
@@ -979,13 +979,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1078,7 +1077,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1258,10 +1257,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1620,7 +1619,7 @@
   <dimension ref="A1:L467"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H470" sqref="H470"/>
+      <selection activeCell="D20" sqref="D20:D464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2408,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="18">
         <v>19</v>
@@ -2449,7 +2448,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="18">
         <v>20</v>
@@ -2489,7 +2488,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="18">
         <v>21</v>
@@ -2529,7 +2528,7 @@
         <v>32</v>
       </c>
       <c r="D23" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="18">
         <v>22</v>
@@ -4088,8 +4087,8 @@
       <c r="C62" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D62" s="42">
-        <v>0</v>
+      <c r="D62" s="38">
+        <v>1</v>
       </c>
       <c r="E62" s="18">
         <v>13</v>
@@ -4128,8 +4127,8 @@
       <c r="C63" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="42">
-        <v>0</v>
+      <c r="D63" s="38">
+        <v>1</v>
       </c>
       <c r="E63" s="18">
         <v>14</v>
@@ -4168,8 +4167,8 @@
       <c r="C64" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="42">
-        <v>0</v>
+      <c r="D64" s="38">
+        <v>1</v>
       </c>
       <c r="E64" s="18">
         <v>15</v>
@@ -4208,8 +4207,8 @@
       <c r="C65" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="42">
-        <v>0</v>
+      <c r="D65" s="38">
+        <v>1</v>
       </c>
       <c r="E65" s="18">
         <v>16</v>
@@ -5128,8 +5127,8 @@
       <c r="C88" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D88" s="15">
-        <v>0</v>
+      <c r="D88" s="38">
+        <v>1</v>
       </c>
       <c r="E88" s="18">
         <v>21</v>
@@ -5168,8 +5167,8 @@
       <c r="C89" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="15">
-        <v>0</v>
+      <c r="D89" s="38">
+        <v>1</v>
       </c>
       <c r="E89" s="18">
         <v>22</v>
@@ -5208,8 +5207,8 @@
       <c r="C90" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D90" s="15">
-        <v>0</v>
+      <c r="D90" s="38">
+        <v>1</v>
       </c>
       <c r="E90" s="18">
         <v>23</v>
@@ -5248,8 +5247,8 @@
       <c r="C91" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D91" s="15">
-        <v>0</v>
+      <c r="D91" s="38">
+        <v>1</v>
       </c>
       <c r="E91" s="18">
         <v>24</v>
@@ -6208,8 +6207,8 @@
       <c r="C115" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D115" s="15">
-        <v>0</v>
+      <c r="D115" s="38">
+        <v>1</v>
       </c>
       <c r="E115" s="18">
         <v>22</v>
@@ -6248,8 +6247,8 @@
       <c r="C116" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D116" s="15">
-        <v>0</v>
+      <c r="D116" s="38">
+        <v>1</v>
       </c>
       <c r="E116" s="18">
         <v>23</v>
@@ -6288,8 +6287,8 @@
       <c r="C117" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D117" s="15">
-        <v>0</v>
+      <c r="D117" s="38">
+        <v>1</v>
       </c>
       <c r="E117" s="18">
         <v>24</v>
@@ -6328,8 +6327,8 @@
       <c r="C118" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D118" s="15">
-        <v>0</v>
+      <c r="D118" s="38">
+        <v>1</v>
       </c>
       <c r="E118" s="18">
         <v>25</v>
@@ -7288,8 +7287,8 @@
       <c r="C142" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D142" s="15">
-        <v>0</v>
+      <c r="D142" s="38">
+        <v>1</v>
       </c>
       <c r="E142" s="18">
         <v>22</v>
@@ -7328,8 +7327,8 @@
       <c r="C143" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D143" s="15">
-        <v>0</v>
+      <c r="D143" s="38">
+        <v>1</v>
       </c>
       <c r="E143" s="18">
         <v>23</v>
@@ -7368,8 +7367,8 @@
       <c r="C144" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D144" s="15">
-        <v>0</v>
+      <c r="D144" s="38">
+        <v>1</v>
       </c>
       <c r="E144" s="18">
         <v>24</v>
@@ -7408,8 +7407,8 @@
       <c r="C145" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D145" s="15">
-        <v>0</v>
+      <c r="D145" s="38">
+        <v>1</v>
       </c>
       <c r="E145" s="18">
         <v>25</v>
@@ -7565,8 +7564,8 @@
       <c r="C149" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D149" s="15">
-        <v>0</v>
+      <c r="D149" s="38">
+        <v>1</v>
       </c>
       <c r="E149" s="18">
         <v>2</v>
@@ -7602,8 +7601,8 @@
       <c r="C150" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D150" s="15">
-        <v>0</v>
+      <c r="D150" s="38">
+        <v>1</v>
       </c>
       <c r="E150" s="18">
         <v>3</v>
@@ -7639,8 +7638,8 @@
       <c r="C151" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D151" s="15">
-        <v>0</v>
+      <c r="D151" s="38">
+        <v>1</v>
       </c>
       <c r="E151" s="18">
         <v>4</v>
@@ -7676,8 +7675,8 @@
       <c r="C152" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D152" s="15">
-        <v>0</v>
+      <c r="D152" s="38">
+        <v>1</v>
       </c>
       <c r="E152" s="18">
         <v>5</v>
@@ -8751,8 +8750,8 @@
       <c r="C180" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D180" s="15">
-        <v>0</v>
+      <c r="D180" s="38">
+        <v>1</v>
       </c>
       <c r="E180" s="18">
         <v>14</v>
@@ -8951,8 +8950,8 @@
       <c r="C185" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D185" s="15">
-        <v>0</v>
+      <c r="D185" s="38">
+        <v>1</v>
       </c>
       <c r="E185" s="18">
         <v>19</v>
@@ -8991,8 +8990,8 @@
       <c r="C186" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D186" s="15">
-        <v>0</v>
+      <c r="D186" s="38">
+        <v>1</v>
       </c>
       <c r="E186" s="18">
         <v>20</v>
@@ -9031,8 +9030,8 @@
       <c r="C187" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D187" s="15">
-        <v>0</v>
+      <c r="D187" s="38">
+        <v>1</v>
       </c>
       <c r="E187" s="18">
         <v>21</v>
@@ -9071,8 +9070,8 @@
       <c r="C188" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D188" s="15">
-        <v>0</v>
+      <c r="D188" s="38">
+        <v>1</v>
       </c>
       <c r="E188" s="18">
         <v>22</v>
@@ -9151,8 +9150,8 @@
       <c r="C190" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D190" s="15">
-        <v>0</v>
+      <c r="D190" s="38">
+        <v>1</v>
       </c>
       <c r="E190" s="18">
         <v>24</v>
@@ -10071,8 +10070,8 @@
       <c r="C213" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D213" s="15">
-        <v>0</v>
+      <c r="D213" s="38">
+        <v>1</v>
       </c>
       <c r="E213" s="18">
         <v>23</v>
@@ -10231,8 +10230,8 @@
       <c r="C217" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D217" s="15">
-        <v>0</v>
+      <c r="D217" s="38">
+        <v>1</v>
       </c>
       <c r="E217" s="18">
         <v>27</v>
@@ -10271,8 +10270,8 @@
       <c r="C218" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D218" s="15">
-        <v>0</v>
+      <c r="D218" s="38">
+        <v>1</v>
       </c>
       <c r="E218" s="18">
         <v>28</v>
@@ -10311,8 +10310,8 @@
       <c r="C219" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D219" s="15">
-        <v>0</v>
+      <c r="D219" s="38">
+        <v>1</v>
       </c>
       <c r="E219" s="18">
         <v>29</v>
@@ -10351,8 +10350,8 @@
       <c r="C220" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D220" s="15">
-        <v>0</v>
+      <c r="D220" s="38">
+        <v>1</v>
       </c>
       <c r="E220" s="18">
         <v>30</v>
@@ -10431,8 +10430,8 @@
       <c r="C222" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D222" s="15">
-        <v>0</v>
+      <c r="D222" s="38">
+        <v>1</v>
       </c>
       <c r="E222" s="18">
         <v>32</v>
@@ -11433,8 +11432,8 @@
       <c r="C249" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D249" s="15">
-        <v>0</v>
+      <c r="D249" s="38">
+        <v>1</v>
       </c>
       <c r="E249" s="18">
         <v>14</v>
@@ -11470,8 +11469,8 @@
       <c r="C250" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D250" s="15">
-        <v>0</v>
+      <c r="D250" s="38">
+        <v>1</v>
       </c>
       <c r="E250" s="18">
         <v>15</v>
@@ -11507,8 +11506,8 @@
       <c r="C251" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D251" s="15">
-        <v>0</v>
+      <c r="D251" s="38">
+        <v>1</v>
       </c>
       <c r="E251" s="18">
         <v>16</v>
@@ -11544,8 +11543,8 @@
       <c r="C252" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D252" s="15">
-        <v>0</v>
+      <c r="D252" s="38">
+        <v>1</v>
       </c>
       <c r="E252" s="18">
         <v>17</v>
@@ -12099,8 +12098,8 @@
       <c r="C267" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D267" s="15">
-        <v>0</v>
+      <c r="D267" s="38">
+        <v>1</v>
       </c>
       <c r="E267" s="18">
         <v>13</v>
@@ -12247,8 +12246,8 @@
       <c r="C271" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D271" s="15">
-        <v>0</v>
+      <c r="D271" s="38">
+        <v>1</v>
       </c>
       <c r="E271" s="18">
         <v>17</v>
@@ -12321,8 +12320,8 @@
       <c r="C273" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D273" s="15">
-        <v>0</v>
+      <c r="D273" s="38">
+        <v>1</v>
       </c>
       <c r="E273" s="18">
         <v>19</v>
@@ -12358,8 +12357,8 @@
       <c r="C274" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D274" s="15">
-        <v>0</v>
+      <c r="D274" s="38">
+        <v>1</v>
       </c>
       <c r="E274" s="18">
         <v>20</v>
@@ -12395,8 +12394,8 @@
       <c r="C275" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D275" s="15">
-        <v>0</v>
+      <c r="D275" s="38">
+        <v>1</v>
       </c>
       <c r="E275" s="18">
         <v>21</v>
@@ -12432,8 +12431,8 @@
       <c r="C276" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D276" s="15">
-        <v>0</v>
+      <c r="D276" s="38">
+        <v>1</v>
       </c>
       <c r="E276" s="18">
         <v>22</v>
@@ -12506,8 +12505,8 @@
       <c r="C278" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D278" s="15">
-        <v>0</v>
+      <c r="D278" s="38">
+        <v>1</v>
       </c>
       <c r="E278" s="18">
         <v>24</v>
@@ -13423,8 +13422,8 @@
       <c r="C301" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D301" s="15">
-        <v>0</v>
+      <c r="D301" s="38">
+        <v>1</v>
       </c>
       <c r="E301" s="18">
         <v>23</v>
@@ -13583,8 +13582,8 @@
       <c r="C305" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D305" s="15">
-        <v>0</v>
+      <c r="D305" s="38">
+        <v>1</v>
       </c>
       <c r="E305" s="18">
         <v>27</v>
@@ -13623,8 +13622,8 @@
       <c r="C306" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D306" s="15">
-        <v>0</v>
+      <c r="D306" s="38">
+        <v>1</v>
       </c>
       <c r="E306" s="18">
         <v>28</v>
@@ -13663,8 +13662,8 @@
       <c r="C307" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D307" s="15">
-        <v>0</v>
+      <c r="D307" s="38">
+        <v>1</v>
       </c>
       <c r="E307" s="18">
         <v>29</v>
@@ -13703,8 +13702,8 @@
       <c r="C308" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D308" s="15">
-        <v>0</v>
+      <c r="D308" s="38">
+        <v>1</v>
       </c>
       <c r="E308" s="18">
         <v>30</v>
@@ -13823,8 +13822,8 @@
       <c r="C311" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D311" s="15">
-        <v>0</v>
+      <c r="D311" s="38">
+        <v>1</v>
       </c>
       <c r="E311" s="18">
         <v>33</v>
@@ -13863,8 +13862,8 @@
       <c r="C312" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D312" s="4">
-        <v>0</v>
+      <c r="D312" s="38">
+        <v>1</v>
       </c>
       <c r="E312" s="18">
         <v>1</v>
@@ -14381,8 +14380,8 @@
       <c r="C326" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D326" s="15">
-        <v>0</v>
+      <c r="D326" s="38">
+        <v>1</v>
       </c>
       <c r="E326" s="18">
         <v>15</v>
@@ -14492,8 +14491,8 @@
       <c r="C329" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D329" s="15">
-        <v>0</v>
+      <c r="D329" s="38">
+        <v>1</v>
       </c>
       <c r="E329" s="18">
         <v>18</v>
@@ -14529,8 +14528,8 @@
       <c r="C330" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D330" s="15">
-        <v>0</v>
+      <c r="D330" s="38">
+        <v>1</v>
       </c>
       <c r="E330" s="18">
         <v>19</v>
@@ -14566,8 +14565,8 @@
       <c r="C331" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D331" s="15">
-        <v>0</v>
+      <c r="D331" s="38">
+        <v>1</v>
       </c>
       <c r="E331" s="18">
         <v>20</v>
@@ -14603,8 +14602,8 @@
       <c r="C332" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D332" s="15">
-        <v>0</v>
+      <c r="D332" s="38">
+        <v>1</v>
       </c>
       <c r="E332" s="18">
         <v>21</v>
@@ -14677,8 +14676,8 @@
       <c r="C334" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D334" s="15">
-        <v>0</v>
+      <c r="D334" s="38">
+        <v>1</v>
       </c>
       <c r="E334" s="18">
         <v>23</v>
@@ -14754,8 +14753,8 @@
       <c r="C336" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D336" s="15">
-        <v>0</v>
+      <c r="D336" s="38">
+        <v>1</v>
       </c>
       <c r="E336" s="18">
         <v>2</v>
@@ -14874,8 +14873,8 @@
       <c r="C339" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D339" s="15">
-        <v>0</v>
+      <c r="D339" s="38">
+        <v>1</v>
       </c>
       <c r="E339" s="18">
         <v>5</v>
@@ -14914,8 +14913,8 @@
       <c r="C340" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D340" s="15">
-        <v>0</v>
+      <c r="D340" s="38">
+        <v>1</v>
       </c>
       <c r="E340" s="18">
         <v>6</v>
@@ -14954,8 +14953,8 @@
       <c r="C341" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D341" s="15">
-        <v>0</v>
+      <c r="D341" s="38">
+        <v>1</v>
       </c>
       <c r="E341" s="18">
         <v>7</v>
@@ -14994,8 +14993,8 @@
       <c r="C342" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D342" s="15">
-        <v>0</v>
+      <c r="D342" s="38">
+        <v>1</v>
       </c>
       <c r="E342" s="18">
         <v>8</v>
@@ -15034,8 +15033,8 @@
       <c r="C343" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D343" s="15">
-        <v>0</v>
+      <c r="D343" s="38">
+        <v>1</v>
       </c>
       <c r="E343" s="18">
         <v>9</v>
@@ -15114,8 +15113,8 @@
       <c r="C345" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="D345" s="15">
-        <v>0</v>
+      <c r="D345" s="38">
+        <v>1</v>
       </c>
       <c r="E345" s="18">
         <v>11</v>
@@ -15474,8 +15473,8 @@
       <c r="C354" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D354" s="15">
-        <v>0</v>
+      <c r="D354" s="38">
+        <v>1</v>
       </c>
       <c r="E354" s="18">
         <v>9</v>
@@ -15554,8 +15553,8 @@
       <c r="C356" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D356" s="15">
-        <v>0</v>
+      <c r="D356" s="38">
+        <v>1</v>
       </c>
       <c r="E356" s="18">
         <v>11</v>
@@ -15594,8 +15593,8 @@
       <c r="C357" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D357" s="15">
-        <v>0</v>
+      <c r="D357" s="38">
+        <v>1</v>
       </c>
       <c r="E357" s="18">
         <v>12</v>
@@ -15634,8 +15633,8 @@
       <c r="C358" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D358" s="15">
-        <v>0</v>
+      <c r="D358" s="38">
+        <v>1</v>
       </c>
       <c r="E358" s="18">
         <v>13</v>
@@ -15674,8 +15673,8 @@
       <c r="C359" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D359" s="15">
-        <v>0</v>
+      <c r="D359" s="38">
+        <v>1</v>
       </c>
       <c r="E359" s="18">
         <v>14</v>
@@ -16164,8 +16163,8 @@
       <c r="C372" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="D372" s="15">
-        <v>0</v>
+      <c r="D372" s="38">
+        <v>1</v>
       </c>
       <c r="E372" s="18">
         <v>11</v>
@@ -16201,8 +16200,8 @@
       <c r="C373" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="D373" s="15">
-        <v>0</v>
+      <c r="D373" s="38">
+        <v>1</v>
       </c>
       <c r="E373" s="18">
         <v>12</v>
@@ -16238,8 +16237,8 @@
       <c r="C374" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="D374" s="15">
-        <v>0</v>
+      <c r="D374" s="38">
+        <v>1</v>
       </c>
       <c r="E374" s="18">
         <v>13</v>
@@ -16275,8 +16274,8 @@
       <c r="C375" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="D375" s="15">
-        <v>0</v>
+      <c r="D375" s="38">
+        <v>1</v>
       </c>
       <c r="E375" s="18">
         <v>14</v>
@@ -16349,8 +16348,8 @@
       <c r="C377" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="D377" s="15">
-        <v>0</v>
+      <c r="D377" s="38">
+        <v>1</v>
       </c>
       <c r="E377" s="18">
         <v>16</v>
@@ -17026,8 +17025,8 @@
       <c r="C394" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D394" s="15">
-        <v>0</v>
+      <c r="D394" s="38">
+        <v>1</v>
       </c>
       <c r="E394" s="18">
         <v>17</v>
@@ -17066,8 +17065,8 @@
       <c r="C395" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D395" s="15">
-        <v>0</v>
+      <c r="D395" s="38">
+        <v>1</v>
       </c>
       <c r="E395" s="18">
         <v>18</v>
@@ -17106,8 +17105,8 @@
       <c r="C396" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D396" s="15">
-        <v>0</v>
+      <c r="D396" s="38">
+        <v>1</v>
       </c>
       <c r="E396" s="18">
         <v>19</v>
@@ -17146,8 +17145,8 @@
       <c r="C397" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D397" s="15">
-        <v>0</v>
+      <c r="D397" s="38">
+        <v>1</v>
       </c>
       <c r="E397" s="18">
         <v>20</v>
@@ -17304,8 +17303,8 @@
       <c r="C401" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="D401" s="15">
-        <v>0</v>
+      <c r="D401" s="38">
+        <v>1</v>
       </c>
       <c r="E401" s="18">
         <v>2</v>
@@ -17342,8 +17341,8 @@
       <c r="C402" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="D402" s="15">
-        <v>0</v>
+      <c r="D402" s="38">
+        <v>1</v>
       </c>
       <c r="E402" s="18">
         <v>3</v>
@@ -17380,8 +17379,8 @@
       <c r="C403" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="D403" s="15">
-        <v>0</v>
+      <c r="D403" s="38">
+        <v>1</v>
       </c>
       <c r="E403" s="18">
         <v>4</v>
@@ -17418,8 +17417,8 @@
       <c r="C404" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="D404" s="15">
-        <v>0</v>
+      <c r="D404" s="38">
+        <v>1</v>
       </c>
       <c r="E404" s="18">
         <v>5</v>
@@ -18412,8 +18411,8 @@
       <c r="C429" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="D429" s="15">
-        <v>0</v>
+      <c r="D429" s="38">
+        <v>1</v>
       </c>
       <c r="E429" s="18">
         <v>23</v>
@@ -18452,8 +18451,8 @@
       <c r="C430" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="D430" s="15">
-        <v>0</v>
+      <c r="D430" s="38">
+        <v>1</v>
       </c>
       <c r="E430" s="18">
         <v>24</v>
@@ -18492,8 +18491,8 @@
       <c r="C431" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="D431" s="15">
-        <v>0</v>
+      <c r="D431" s="38">
+        <v>1</v>
       </c>
       <c r="E431" s="18">
         <v>25</v>
@@ -18532,8 +18531,8 @@
       <c r="C432" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="D432" s="15">
-        <v>0</v>
+      <c r="D432" s="38">
+        <v>1</v>
       </c>
       <c r="E432" s="18">
         <v>26</v>
@@ -18689,8 +18688,8 @@
       <c r="C436" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="D436" s="15">
-        <v>0</v>
+      <c r="D436" s="38">
+        <v>1</v>
       </c>
       <c r="E436" s="18">
         <v>2</v>
@@ -18726,8 +18725,8 @@
       <c r="C437" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="D437" s="15">
-        <v>0</v>
+      <c r="D437" s="38">
+        <v>1</v>
       </c>
       <c r="E437" s="18">
         <v>3</v>
@@ -18763,8 +18762,8 @@
       <c r="C438" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="D438" s="15">
-        <v>0</v>
+      <c r="D438" s="38">
+        <v>1</v>
       </c>
       <c r="E438" s="18">
         <v>4</v>
@@ -18800,8 +18799,8 @@
       <c r="C439" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="D439" s="15">
-        <v>0</v>
+      <c r="D439" s="38">
+        <v>1</v>
       </c>
       <c r="E439" s="18">
         <v>5</v>
@@ -19671,8 +19670,8 @@
       <c r="C461" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D461" s="15">
-        <v>0</v>
+      <c r="D461" s="38">
+        <v>1</v>
       </c>
       <c r="E461" s="18">
         <v>20</v>
@@ -19711,8 +19710,8 @@
       <c r="C462" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D462" s="15">
-        <v>0</v>
+      <c r="D462" s="38">
+        <v>1</v>
       </c>
       <c r="E462" s="18">
         <v>21</v>
@@ -19751,8 +19750,8 @@
       <c r="C463" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D463" s="15">
-        <v>0</v>
+      <c r="D463" s="38">
+        <v>1</v>
       </c>
       <c r="E463" s="18">
         <v>22</v>
@@ -19791,8 +19790,8 @@
       <c r="C464" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D464" s="15">
-        <v>0</v>
+      <c r="D464" s="38">
+        <v>1</v>
       </c>
       <c r="E464" s="18">
         <v>23</v>

</xml_diff>